<commit_message>
added 1-2 solutions and slides
</commit_message>
<xml_diff>
--- a/Module_01-Excel/2-Data_Fundamentals_in_Excel/03-Ins_ColorCounter/Solved/FavoriteColors.xlsx
+++ b/Module_01-Excel/2-Data_Fundamentals_in_Excel/03-Ins_ColorCounter/Solved/FavoriteColors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcorless/Documents/coding-boot-camp/DataViz-Lesson-Plans/01-Lesson-Plans/01-Excel/2/Activities/03-Ins_ColorCounter/Solved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/Documents/Personal/Career/Work/2U/live_online/class_files/2024_Fall_West_Coast/clean_lecture/DataViz-Lesson-Plans/01-Lesson-Plans/01-Excel/2/Activities/03-Ins_ColorCounter/Solved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46108015-2369-D048-8A0C-F870D2F0C0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264B0244-F4AA-C84B-AC4A-ABA913EAC41C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Favorite Colors" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="Colors">'Favorite Colors'!$A$2:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -237,6 +237,11 @@
       <tableStyleElement type="headerRow" dxfId="6"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF35FB"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -547,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,37 +588,37 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,6),"Red","Blue","Yellow","Green","Purple","Orange")</f>
-        <v>Blue</v>
+        <v>Purple</v>
       </c>
       <c r="C2">
         <f ca="1">COUNTIF(Colors,"Red")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <f ca="1">COUNTIF(Colors,"Blue")</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <f ca="1">COUNTIF(Colors,"Yellow")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <f ca="1">COUNTIF(Colors,"Purple")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G2">
         <f ca="1">COUNTIF(Colors,"Orange")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <f ca="1">COUNTIF(Colors,"Green")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="str">
         <f t="shared" ref="A3:A30" ca="1" si="0">CHOOSE(RANDBETWEEN(1,6),"Red","Blue","Yellow","Green","Purple","Orange")</f>
-        <v>Purple</v>
+        <v>Orange</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -646,15 +651,15 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Green</v>
+        <v>Purple</v>
       </c>
       <c r="C5" t="b">
         <f ca="1">IF(C2&gt;5,TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="b">
         <f t="shared" ref="D5:H5" ca="1" si="1">IF(D2&gt;5,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="b">
         <f t="shared" ca="1" si="1"/>
@@ -680,13 +685,13 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Green</v>
+        <v>Purple</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Purple</v>
+        <v>Green</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -698,25 +703,25 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Red</v>
+        <v>Purple</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Blue</v>
+        <v>Green</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Green</v>
+        <v>Red</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Red</v>
+        <v>Orange</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -728,55 +733,55 @@
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Blue</v>
+        <v>Yellow</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Blue</v>
+        <v>Red</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Purple</v>
+        <v>Green</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Orange</v>
+        <v>Red</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">CHOOSE(RANDBETWEEN(1,6),"Red","Blue","Yellow","Green","Purple","Orange")</f>
         <v>Purple</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yellow</v>
+        <v>Orange</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Orange</v>
+        <v>Red</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Blue</v>
+        <v>Green</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Green</v>
+        <v>Yellow</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
@@ -788,13 +793,13 @@
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Red</v>
+        <v>Yellow</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Orange</v>
+        <v>Blue</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
@@ -806,25 +811,25 @@
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Orange</v>
+        <v>Green</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Blue</v>
+        <v>Red</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Orange</v>
+        <v>Purple</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Blue</v>
+        <v>Purple</v>
       </c>
     </row>
   </sheetData>

</xml_diff>